<commit_message>
rewrite alignment and patch-placer GUIs to use the params JSON for all offset and image parsing information. This lets us set per-image image processing parameters. The whole patches_gui.py is replaced to use the new implementation - much cleaner overall. Patches GUI also allows real-time inputs of processing parameters, and shows the bounding box and processed image for each patch. New test files for both. Temporary client scripts for the align and patch gui will be folded into the existing run scripts - shouldn't be much mismatch.
</commit_message>
<xml_diff>
--- a/tests/dataset_index.xlsx
+++ b/tests/dataset_index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Python\ehd_exsitu\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Python\ehd_exsitu\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966634EB-63FD-4E18-8DAD-60879CECE89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC51035-0677-4CE0-8AE2-84BCAD22D0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="3645" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -385,7 +385,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
** changed scikit pipe from self.model to self.pipe - only 2 levels of self.model nesting overload now. ** Wrote test script test_ehd_model.py ** Updated test dataset to reflect new columns ** Implemented save/load functionality to EHD_Model ** Cleaned up unused normalized_input_models.py ** Created hyperparam tuning loop using Ray.tune in model_tuner.py ** New entry point script tune.py to tune hyperparameters - hyperparam loop seems to basically work! ** Renamed EHD_Model.model.model to pipe. (It's usually a scikitlearn pipeline in the model wrapper) ** Listed hyperparameters for RF_Classifier_Allpre - added check to set max_samples=None if bootstrapping is off.
</commit_message>
<xml_diff>
--- a/tests/dataset_index.xlsx
+++ b/tests/dataset_index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Python\ehd_exsitu\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC51035-0677-4CE0-8AE2-84BCAD22D0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6B087D-0BCE-4B9B-A15F-C3F66EDBCD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="3645" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Path</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>harmonics</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>V Thresh [V] @ .5s</t>
+  </si>
+  <si>
+    <t>W thresh [s] @ 1.5 Vt</t>
   </si>
 </sst>
 </file>
@@ -382,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G1" sqref="G1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,7 +404,7 @@
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +423,17 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -433,6 +451,9 @@
       </c>
       <c r="F2">
         <v>570</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>